<commit_message>
fix some issues reported by data consumer
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D23954-2A4E-FD47-8AFB-A3C9CE0B6E9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39101A2B-CA3E-BF43-93F6-38F78FBC7F26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>门店</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>别名</t>
+  </si>
+  <si>
+    <t>评价激励达标</t>
   </si>
 </sst>
 </file>
@@ -690,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -701,11 +704,12 @@
     <col min="1" max="1" width="68.796875" customWidth="1"/>
     <col min="2" max="2" width="42.19921875" customWidth="1"/>
     <col min="3" max="3" width="26.19921875" customWidth="1"/>
-    <col min="4" max="4" width="17.59765625" customWidth="1"/>
-    <col min="5" max="5" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="33.796875" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickTop="1">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" thickTop="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -719,10 +723,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -736,10 +743,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E2" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F2" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -753,10 +763,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E3" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -770,10 +783,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E4" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -787,10 +803,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E5" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -804,10 +823,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E6" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -821,10 +843,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E7" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -838,10 +863,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E8" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -855,10 +883,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E9" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -872,10 +903,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E10" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -889,10 +923,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E11" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -906,10 +943,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E12" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -920,13 +960,16 @@
         <v>44</v>
       </c>
       <c r="D13" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E13" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -940,10 +983,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E14" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -957,10 +1003,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E15" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -974,10 +1023,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E16" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -991,10 +1043,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E17" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1005,13 +1060,16 @@
         <v>44</v>
       </c>
       <c r="D18" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E18" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1025,10 +1083,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E19" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F19" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1042,10 +1103,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E20" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F20" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1059,10 +1123,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E21" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F21" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1076,10 +1143,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E22" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F22" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1093,10 +1163,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E23" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1110,10 +1183,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E24" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F24" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1127,10 +1203,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E25" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F25" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1144,10 +1223,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E26" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F26" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1161,10 +1243,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E27" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1178,10 +1263,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E28" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F28" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1195,10 +1283,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E29" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F29" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1212,10 +1303,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E30" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1229,10 +1323,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E31" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
@@ -1246,10 +1343,13 @@
         <v>4.5</v>
       </c>
       <c r="E32" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F32" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1263,10 +1363,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E33" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F33" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1280,10 +1383,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E34" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1297,10 +1403,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E35" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="18.75" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
@@ -1313,11 +1422,14 @@
       <c r="D36" s="5">
         <v>4.5</v>
       </c>
-      <c r="E36" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="18.75" customHeight="1">
+      <c r="E36" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F36" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18.75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1331,10 +1443,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E37" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="18.75" customHeight="1">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
@@ -1347,11 +1462,14 @@
       <c r="D38" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F38" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="18.75" customHeight="1">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
@@ -1364,11 +1482,14 @@
       <c r="D39" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F39" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="18.75" customHeight="1">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -1382,6 +1503,9 @@
         <v>4.5</v>
       </c>
       <c r="E40" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F40" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hand the special case 三峡广场店
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/daily_motivate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/liziba_daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39101A2B-CA3E-BF43-93F6-38F78FBC7F26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A2EE9-DF42-D142-AADC-E90E2C26F627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT_SHEET" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>门店</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>受气牛肉解放碑店</t>
-  </si>
-  <si>
-    <t>李子坝梁山鸡三峡广场店</t>
   </si>
   <si>
     <t>李子坝梁山鸡东原悦荟店</t>
@@ -693,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -714,16 +711,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -737,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2">
         <v>4.5999999999999996</v>
@@ -757,7 +754,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>4.5999999999999996</v>
@@ -777,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>4.5999999999999996</v>
@@ -790,14 +787,14 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2">
         <v>4.5999999999999996</v>
@@ -817,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
         <v>4.5999999999999996</v>
@@ -837,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2">
         <v>4.5999999999999996</v>
@@ -857,7 +854,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2">
         <v>4.5999999999999996</v>
@@ -877,7 +874,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <v>4.5999999999999996</v>
@@ -897,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2">
         <v>4.5999999999999996</v>
@@ -917,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2">
         <v>4.5999999999999996</v>
@@ -937,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>4.5999999999999996</v>
@@ -957,7 +954,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
         <v>4.5999999999999996</v>
@@ -977,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
         <v>4.5999999999999996</v>
@@ -997,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2">
         <v>4.5999999999999996</v>
@@ -1017,7 +1014,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2">
         <v>4.5999999999999996</v>
@@ -1037,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2">
         <v>4.5999999999999996</v>
@@ -1057,7 +1054,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2">
         <v>4.5999999999999996</v>
@@ -1077,7 +1074,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
         <v>4.5999999999999996</v>
@@ -1097,7 +1094,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2">
         <v>4.5999999999999996</v>
@@ -1110,14 +1107,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2">
         <v>4.5999999999999996</v>
@@ -1137,7 +1134,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
         <v>4.5999999999999996</v>
@@ -1146,7 +1143,7 @@
         <v>4.8</v>
       </c>
       <c r="F22" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
@@ -1157,7 +1154,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2">
         <v>4.5999999999999996</v>
@@ -1166,7 +1163,7 @@
         <v>4.8</v>
       </c>
       <c r="F23" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1">
@@ -1177,7 +1174,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2">
         <v>4.5999999999999996</v>
@@ -1197,7 +1194,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2">
         <v>4.5999999999999996</v>
@@ -1217,7 +1214,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <v>4.5999999999999996</v>
@@ -1237,7 +1234,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="2">
         <v>4.5999999999999996</v>
@@ -1257,7 +1254,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2">
         <v>4.5999999999999996</v>
@@ -1266,7 +1263,7 @@
         <v>4.8</v>
       </c>
       <c r="F28" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1">
@@ -1277,7 +1274,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2">
         <v>4.5999999999999996</v>
@@ -1286,7 +1283,7 @@
         <v>4.8</v>
       </c>
       <c r="F29" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1">
@@ -1297,7 +1294,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="2">
         <v>4.5999999999999996</v>
@@ -1306,41 +1303,41 @@
         <v>4.8</v>
       </c>
       <c r="F30" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F31" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E31" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F31" s="2">
-        <v>7</v>
-      </c>
-    </row>
     <row r="32" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E32" s="2">
         <v>4.8</v>
@@ -1357,7 +1354,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="2">
         <v>4.5999999999999996</v>
@@ -1377,7 +1374,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="2">
         <v>4.5999999999999996</v>
@@ -1390,17 +1387,17 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
+      <c r="A35" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="2">
-        <v>4.5999999999999996</v>
+        <v>44</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4.5</v>
       </c>
       <c r="E35" s="2">
         <v>4.8</v>
@@ -1410,17 +1407,17 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A36" s="4" t="s">
-        <v>41</v>
+      <c r="A36" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="5">
-        <v>4.5</v>
+        <v>44</v>
+      </c>
+      <c r="D36" s="2">
+        <v>4.5999999999999996</v>
       </c>
       <c r="E36" s="2">
         <v>4.8</v>
@@ -1430,23 +1427,23 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="5">
         <v>4.5999999999999996</v>
       </c>
       <c r="E37" s="2">
         <v>4.8</v>
       </c>
-      <c r="F37" s="2">
-        <v>6</v>
+      <c r="F37" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1">
@@ -1470,42 +1467,22 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="5">
-        <v>4.5999999999999996</v>
+      <c r="C39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4.5</v>
       </c>
       <c r="E39" s="2">
         <v>4.8</v>
       </c>
-      <c r="F39" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E40" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F40" s="2">
+      <c r="F39" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rules changes according to operation requirements
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/liziba_daily_motivate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A2EE9-DF42-D142-AADC-E90E2C26F627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1670614B-488E-5C44-8C01-1F35DC34B694}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" xWindow="6600" yWindow="3080" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT_SHEET" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
   <si>
     <t>门店</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>评价激励达标</t>
+  </si>
+  <si>
+    <t>李子坝梁山鸡约克郡光环店</t>
+  </si>
+  <si>
+    <t>受气牛肉约克郡光环店</t>
   </si>
 </sst>
 </file>
@@ -690,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -1087,7 +1093,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1107,17 +1113,17 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>22</v>
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="E21" s="2">
         <v>4.8</v>
@@ -1128,10 +1134,10 @@
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>44</v>
@@ -1143,15 +1149,15 @@
         <v>4.8</v>
       </c>
       <c r="F22" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>44</v>
@@ -1163,15 +1169,15 @@
         <v>4.8</v>
       </c>
       <c r="F23" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>44</v>
@@ -1188,10 +1194,10 @@
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>44</v>
@@ -1208,10 +1214,10 @@
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>44</v>
@@ -1228,10 +1234,10 @@
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>44</v>
@@ -1248,10 +1254,10 @@
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>44</v>
@@ -1263,15 +1269,15 @@
         <v>4.8</v>
       </c>
       <c r="F28" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>44</v>
@@ -1283,61 +1289,61 @@
         <v>4.8</v>
       </c>
       <c r="F29" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E30" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="C31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F31" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2">
         <v>4.5</v>
-      </c>
-      <c r="E31" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F31" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="2">
-        <v>4.5999999999999996</v>
       </c>
       <c r="E32" s="2">
         <v>4.8</v>
@@ -1348,10 +1354,10 @@
     </row>
     <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>44</v>
@@ -1368,121 +1374,161 @@
     </row>
     <row r="34" spans="1:6" ht="18.75" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E34" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F34" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A35" s="4" t="s">
+      <c r="C35" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="5">
+      <c r="C36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="5">
         <v>4.5</v>
       </c>
-      <c r="E35" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F35" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A36" s="1" t="s">
+      <c r="E36" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F36" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E36" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F36" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A37" s="4" t="s">
+      <c r="C37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F38" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E37" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F37" s="5">
+      <c r="D39" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F39" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E38" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F38" s="5">
+      <c r="D40" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E40" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F40" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A39" s="3" t="s">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D41" s="2">
         <v>4.5</v>
       </c>
-      <c r="E39" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="E41" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F41" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new stores are added
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/liziba_daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C2D368-D827-7545-BD62-5E8487C42713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5304A0-4B34-FC46-AB5A-D03881F1234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
   <si>
     <t>门店</t>
   </si>
@@ -181,14 +181,26 @@
     <t>李子坝梁山鸡万象汇店</t>
   </si>
   <si>
+    <t>李子坝梁山鸡大渡口万象汇店</t>
+  </si>
+  <si>
     <t>受气牛肉万象汇店</t>
+  </si>
+  <si>
+    <t>受气牛肉大渡口万象汇店</t>
+  </si>
+  <si>
+    <t>受气牛肉李子坝旗舰店</t>
+  </si>
+  <si>
+    <t>受气牛肉李子坝店</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -210,6 +222,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -355,7 +373,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -396,6 +414,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -702,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -713,7 +737,7 @@
     <col min="1" max="1" width="68.796875" customWidth="1"/>
     <col min="2" max="2" width="42.19921875" customWidth="1"/>
     <col min="3" max="3" width="26.19921875" customWidth="1"/>
-    <col min="4" max="4" width="33.796875" customWidth="1"/>
+    <col min="4" max="4" width="24.796875" customWidth="1"/>
     <col min="5" max="5" width="20.59765625" customWidth="1"/>
     <col min="6" max="6" width="12.59765625" customWidth="1"/>
   </cols>
@@ -1140,10 +1164,10 @@
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>43</v>
@@ -1155,35 +1179,35 @@
         <v>4.8</v>
       </c>
       <c r="F22" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>22</v>
+      <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="E23" s="2">
         <v>4.8</v>
       </c>
       <c r="F23" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>44</v>
@@ -1195,15 +1219,15 @@
         <v>4.8</v>
       </c>
       <c r="F24" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>44</v>
@@ -1215,15 +1239,15 @@
         <v>4.8</v>
       </c>
       <c r="F25" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>44</v>
@@ -1240,10 +1264,10 @@
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>44</v>
@@ -1260,10 +1284,10 @@
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>44</v>
@@ -1280,10 +1304,10 @@
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>44</v>
@@ -1300,10 +1324,10 @@
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>44</v>
@@ -1315,15 +1339,15 @@
         <v>4.8</v>
       </c>
       <c r="F30" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>44</v>
@@ -1335,61 +1359,61 @@
         <v>4.8</v>
       </c>
       <c r="F31" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E32" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F32" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E32" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F32" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A33" s="3" t="s">
+      <c r="C33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F33" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="2">
         <v>4.5</v>
-      </c>
-      <c r="E33" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F33" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="2">
-        <v>4.5999999999999996</v>
       </c>
       <c r="E34" s="2">
         <v>4.8</v>
@@ -1400,10 +1424,10 @@
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>44</v>
@@ -1420,10 +1444,10 @@
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>44</v>
@@ -1439,17 +1463,17 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A37" s="4" t="s">
-        <v>40</v>
+      <c r="A37" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="5">
-        <v>4.5</v>
+      <c r="D37" s="2">
+        <v>4.5999999999999996</v>
       </c>
       <c r="E37" s="2">
         <v>4.8</v>
@@ -1459,17 +1483,17 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>36</v>
+      <c r="A38" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="2">
-        <v>4.5999999999999996</v>
+        <v>40</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4.5</v>
       </c>
       <c r="E38" s="2">
         <v>4.8</v>
@@ -1479,17 +1503,17 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A39" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>50</v>
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E39" s="2">
         <v>4.8</v>
@@ -1500,10 +1524,10 @@
     </row>
     <row r="40" spans="1:6" ht="18.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>44</v>
@@ -1519,62 +1543,82 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="5">
-        <v>4.5999999999999996</v>
+      <c r="A41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="2">
+        <v>4.5</v>
       </c>
       <c r="E41" s="2">
         <v>4.8</v>
       </c>
-      <c r="F41" s="5">
-        <v>7</v>
+      <c r="F41" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18.75" customHeight="1">
       <c r="A42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E42" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F42" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E42" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F42" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A43" s="3" t="s">
+      <c r="D43" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F43" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A44" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D44" s="2">
         <v>4.5</v>
       </c>
-      <c r="E43" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="E44" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F44" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix the exception when di is empty
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/liziba_daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5304A0-4B34-FC46-AB5A-D03881F1234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD08517-6A23-7F4B-A624-4EB0E6F6E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="61">
   <si>
     <t>门店</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>受气牛肉李子坝店</t>
+  </si>
+  <si>
+    <t>受气牛肉巴南万达店</t>
+  </si>
+  <si>
+    <t>李子坝梁山鸡巴南万达店</t>
+  </si>
+  <si>
+    <t>李子坝梁山鸡昆明南亚首店</t>
   </si>
 </sst>
 </file>
@@ -726,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -1189,7 +1198,7 @@
       <c r="B23" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="2">
@@ -1203,31 +1212,31 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>44</v>
+      <c r="A24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D24" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="E24" s="2">
         <v>4.8</v>
       </c>
       <c r="F24" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>44</v>
@@ -1239,15 +1248,15 @@
         <v>4.8</v>
       </c>
       <c r="F25" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>44</v>
@@ -1259,15 +1268,15 @@
         <v>4.8</v>
       </c>
       <c r="F26" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>44</v>
@@ -1284,10 +1293,10 @@
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>44</v>
@@ -1304,10 +1313,10 @@
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>44</v>
@@ -1324,10 +1333,10 @@
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>44</v>
@@ -1344,10 +1353,10 @@
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>44</v>
@@ -1359,15 +1368,15 @@
         <v>4.8</v>
       </c>
       <c r="F31" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>44</v>
@@ -1379,61 +1388,61 @@
         <v>4.8</v>
       </c>
       <c r="F32" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F33" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E33" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F33" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A34" s="3" t="s">
+      <c r="C34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F34" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C35" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="2">
         <v>4.5</v>
-      </c>
-      <c r="E34" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F34" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="2">
-        <v>4.5999999999999996</v>
       </c>
       <c r="E35" s="2">
         <v>4.8</v>
@@ -1444,10 +1453,10 @@
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>44</v>
@@ -1464,76 +1473,76 @@
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1">
       <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E37" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F37" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A38" s="4" t="s">
+      <c r="C38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E38" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F38" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="5">
+      <c r="C39" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="5">
         <v>4.5</v>
       </c>
-      <c r="E38" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F38" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A39" s="1" t="s">
+      <c r="E39" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F39" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E39" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="F39" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="C40" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="2">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E40" s="2">
         <v>4.8</v>
@@ -1544,10 +1553,10 @@
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>44</v>
@@ -1563,54 +1572,54 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="5">
-        <v>4.5999999999999996</v>
+      <c r="A42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="2">
+        <v>4.5</v>
       </c>
       <c r="E42" s="2">
         <v>4.8</v>
       </c>
-      <c r="F42" s="5">
-        <v>7</v>
+      <c r="F42" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A43" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" s="5">
-        <v>4.5999999999999996</v>
+      <c r="A43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4.5</v>
       </c>
       <c r="E43" s="2">
         <v>4.8</v>
       </c>
-      <c r="F43" s="5">
-        <v>7</v>
+      <c r="F43" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>45</v>
+        <v>60</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="D44" s="2">
         <v>4.5</v>
@@ -1619,6 +1628,66 @@
         <v>4.8</v>
       </c>
       <c r="F44" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E45" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F45" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E46" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F46" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F47" s="2">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new store is added and sql changes
</commit_message>
<xml_diff>
--- a/daily_motivate.xlsx
+++ b/daily_motivate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redlin/Documents/projects/liziba/liziba_daily_motivate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A918DEC-542C-514E-A624-2518571907C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A342F6-BA34-5746-9034-71E02D2CF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT_SHEET" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t>门店</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>受气牛肉观音桥大融城店</t>
+  </si>
+  <si>
+    <t>重渝口味</t>
+  </si>
+  <si>
+    <t>来个宝沸堂蛙</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -379,20 +385,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,13 +427,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,20 +445,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="18.75" customHeight="1"/>
@@ -1714,7 +1749,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="49" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A49" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E49" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F49" s="2">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>